<commit_message>
241211 김동휘  - packaging작업
</commit_message>
<xml_diff>
--- a/src/dh/설계문서.xlsx
+++ b/src/dh/설계문서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\김동휘\workplace\Alpaco10_Final2\src\dh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B633ECC-1E89-4C8B-9917-5B5F3294A2DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51A1E7E-32D3-4CAF-9773-D636A661FE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="110" yWindow="110" windowWidth="19090" windowHeight="9970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DB설계" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,6 +416,26 @@
   </si>
   <si>
     <t>레퍼런스리스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VARCHR(16)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자코드 - 시연에서 P0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.patient_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -506,13 +526,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,7 +631,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -667,6 +687,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
@@ -1124,8 +1147,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A53AA62-9E36-4F11-BCA7-CB66626CDF7B}" name="표1_4" displayName="표1_4" ref="A13:D20" totalsRowShown="0">
-  <autoFilter ref="A13:D20" xr:uid="{1A53AA62-9E36-4F11-BCA7-CB66626CDF7B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A53AA62-9E36-4F11-BCA7-CB66626CDF7B}" name="표1_4" displayName="표1_4" ref="A14:D21" totalsRowShown="0">
+  <autoFilter ref="A14:D21" xr:uid="{1A53AA62-9E36-4F11-BCA7-CB66626CDF7B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4449D490-1106-422D-AE41-796E58E4D4D9}" name="column name"/>
     <tableColumn id="2" xr3:uid="{52B39D48-0FC8-4716-979C-A0E66D8A17A0}" name="type"/>
@@ -1137,8 +1160,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A4:D9" totalsRowShown="0">
-  <autoFilter ref="A4:D9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A4:D10" totalsRowShown="0">
+  <autoFilter ref="A4:D10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="column name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="type"/>
@@ -1150,8 +1173,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EE0471B8-CACC-497B-8CC3-34BDE99A782D}" name="표1_45" displayName="표1_45" ref="A24:D30" totalsRowShown="0">
-  <autoFilter ref="A24:D30" xr:uid="{EE0471B8-CACC-497B-8CC3-34BDE99A782D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EE0471B8-CACC-497B-8CC3-34BDE99A782D}" name="표1_45" displayName="표1_45" ref="A25:D31" totalsRowShown="0">
+  <autoFilter ref="A25:D31" xr:uid="{EE0471B8-CACC-497B-8CC3-34BDE99A782D}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{23E184ED-9C78-485B-B5A6-8E0939EC8B64}" name="column name"/>
     <tableColumn id="2" xr3:uid="{290A4536-2FC7-4D64-BCCA-1FD94A3B585E}" name="type"/>
@@ -1163,8 +1186,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D198FAB2-9549-4702-9CE1-41342D8D0534}" name="표1_456" displayName="표1_456" ref="A34:D40" totalsRowShown="0">
-  <autoFilter ref="A34:D40" xr:uid="{D198FAB2-9549-4702-9CE1-41342D8D0534}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D198FAB2-9549-4702-9CE1-41342D8D0534}" name="표1_456" displayName="표1_456" ref="A35:D41" totalsRowShown="0">
+  <autoFilter ref="A35:D41" xr:uid="{D198FAB2-9549-4702-9CE1-41342D8D0534}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{63CE6F3F-F5F2-4DA1-A932-DF094DAF82CB}" name="column name"/>
     <tableColumn id="2" xr3:uid="{52DC9E89-45FD-4220-8427-9DDC44C4772A}" name="type"/>
@@ -1475,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H40"/>
+  <dimension ref="A2:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1517,169 +1540,167 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="19" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
+      <c r="A7" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" t="s">
-        <v>63</v>
+      <c r="A16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
         <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>54</v>
@@ -1688,227 +1709,232 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.45">
-      <c r="A22" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>70</v>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.45">
+      <c r="A23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>4</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>5</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B26" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="B27" t="s">
         <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
         <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>56</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>57</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>52</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.45">
-      <c r="A32" s="2" t="s">
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.45">
+      <c r="A33" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A35" s="3" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B36" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C36" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
         <v>61</v>
@@ -1916,10 +1942,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
@@ -1927,12 +1953,23 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>89</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>54</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1952,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A12" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>

</xml_diff>